<commit_message>
Atualização dos arquivos de previsão e estoque:
- Modificado: estudo de previsao.xlsx - ajustes nos dados de previsão para melhorar a análise.
- Modificado: zmb51_historico_reduzido.xlsx - atualização do histórico reduzido de inventário para manter a precisão dos dados.
- Modificado: zstok.XLSX - corrigidos os dados de estoque conforme última atualização.
- Novo arquivo: ~$zstok.XLSX - arquivo temporário de backup adicionado.

Essas alterações visam otimizar a consistência e a precisão nas previsões e no controle de estoque.
</commit_message>
<xml_diff>
--- a/Forecast/Arquivos/estudo de previsao.xlsx
+++ b/Forecast/Arquivos/estudo de previsao.xlsx
@@ -2207,8 +2207,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x010100C4D4C92C1AD0124FAEA2CE549EB47725" ma:contentTypeVersion="14" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="f234a2db794dc5e909fa783abeb6acd3">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="650b17bc-3d2f-4f7f-90ed-91d7c74cb221" xmlns:ns3="061e156a-84b8-4e44-9cf1-0142f791148d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="76fd6f4e70c0f14c21b6ef04a53ebb13" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C4D4C92C1AD0124FAEA2CE549EB47725" ma:contentTypeVersion="14" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="5dead4c4ef57c4e73e489df9a16ce9b7">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="650b17bc-3d2f-4f7f-90ed-91d7c74cb221" xmlns:ns3="061e156a-84b8-4e44-9cf1-0142f791148d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b7ecd7c07ef388f6e139b26b0cabd87a" ns2:_="" ns3:_="">
     <xsd:import namespace="650b17bc-3d2f-4f7f-90ed-91d7c74cb221"/>
     <xsd:import namespace="061e156a-84b8-4e44-9cf1-0142f791148d"/>
     <xsd:element name="properties">
@@ -2260,7 +2260,7 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="画像タグ" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="dfbef511-2697-4f49-910f-ca747039f65a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="13" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Marcações de imagem" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="dfbef511-2697-4f49-910f-ca747039f65a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -2309,7 +2309,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="20" nillable="true" ma:displayName="共有相手" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="20" nillable="true" ma:displayName="Compartilhado com" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -2328,7 +2328,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="21" nillable="true" ma:displayName="共有相手の詳細情報" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="21" nillable="true" ma:displayName="Detalhes de Compartilhado Com" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -2345,8 +2345,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="コンテンツ タイプ"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="タイトル"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -2456,22 +2456,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C629FD15-17C6-43F7-B9EB-A12CF08F66B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="650b17bc-3d2f-4f7f-90ed-91d7c74cb221"/>
-    <ds:schemaRef ds:uri="061e156a-84b8-4e44-9cf1-0142f791148d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{948CBF34-0518-4C8B-8297-D2448D7D2607}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>